<commit_message>
feat: add model similarity, trait similarity analysis
</commit_message>
<xml_diff>
--- a/data_for_tree/343taxa_speicies-name_clade-name_color-code.xlsx
+++ b/data_for_tree/343taxa_speicies-name_clade-name_color-code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Google Drive/yeast model update/300 yeast species/0_332yeast_genomes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xluhon/Documents/GitHub/R_code_for_graph_in_evolution/data_for_tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F3EAFD-9216-884F-9F2A-B705937434B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EFCCC5-C533-9343-8C0C-3EBFA1D59FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34300" yWindow="1720" windowWidth="27700" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37040" yWindow="8320" windowWidth="27700" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="343taxa_speicies-name_clade-nam" sheetId="1" r:id="rId1"/>
@@ -4285,7 +4285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4477,6 +4477,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -4638,11 +4644,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5000,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C47" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7494,7 +7501,7 @@
       <c r="C66" t="s">
         <v>277</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="4" t="s">
         <v>278</v>
       </c>
       <c r="E66" t="s">

</xml_diff>